<commit_message>
Two versions of priority added
</commit_message>
<xml_diff>
--- a/cloud_scheduling.xlsx
+++ b/cloud_scheduling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierlim/PycharmProjects/genetic_algorithm_cloud_scheduling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5E2509-80A3-0747-A018-8AD4AC1BEB8C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4657D7-20F3-074B-8800-E373FC35004D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">GA!$C$5:$G$13</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">GA!$C$5:$G$13</definedName>
     <definedName name="solver_lhs4" localSheetId="2" hidden="1">GA!$C$5:$G$13</definedName>
-    <definedName name="solver_lhs5" localSheetId="2" hidden="1">GA!$E$26</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">GA!$E$29</definedName>
     <definedName name="solver_lhs6" localSheetId="2" hidden="1">GA!$M$7:$Q$10</definedName>
     <definedName name="solver_lhs7" localSheetId="2" hidden="1">GA!$M$7:$Q$10</definedName>
     <definedName name="solver_lhs8" localSheetId="2" hidden="1">GA!$R$10:$S$10</definedName>
@@ -45,7 +45,7 @@
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">5</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">GA!$F$29</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">GA!$F$32</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
@@ -71,7 +71,7 @@
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">alldifferent</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">integer</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_rhs5" localSheetId="2" hidden="1">GA!$H$26</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">GA!$H$29</definedName>
     <definedName name="solver_rhs6" localSheetId="2" hidden="1">integer</definedName>
     <definedName name="solver_rhs7" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rhs8" localSheetId="2" hidden="1">42</definedName>
@@ -80,7 +80,7 @@
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">1000</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
@@ -284,7 +284,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
@@ -294,6 +294,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -12798,10 +12799,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A3:W29"/>
+  <dimension ref="A3:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12814,7 +12815,7 @@
     <col min="15" max="15" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
@@ -12834,7 +12835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -12845,7 +12846,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -12866,7 +12867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1">
@@ -12885,7 +12886,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -12906,7 +12907,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
@@ -12925,7 +12926,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1">
@@ -12944,7 +12945,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -12965,7 +12966,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C11" s="1">
         <v>25</v>
       </c>
@@ -12982,7 +12983,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C12" s="1">
         <v>5</v>
       </c>
@@ -12999,7 +13000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C13" s="4">
         <v>41</v>
       </c>
@@ -13016,316 +13017,337 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="18" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="8"/>
-    </row>
-    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="1">
+      <c r="B19" s="5"/>
+      <c r="C19" s="1">
         <f>VLOOKUP(C5,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>0.85</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D19" s="1">
         <f>VLOOKUP(D5,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>0.42</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E19" s="1">
         <f>VLOOKUP(E5,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>0.95</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F19" s="1">
         <f>VLOOKUP(F5,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>0.78</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G19" s="1">
         <f>VLOOKUP(G5,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>0.1</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H19" s="1">
         <f>VLOOKUP(C6,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>0.75</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I19" s="1">
         <f>VLOOKUP(D6,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>0.61</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J19" s="1">
         <f>VLOOKUP(E6,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>0.26</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K19" s="1">
         <f>VLOOKUP(F6,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>0.71</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L19" s="1">
         <f>VLOOKUP(G6,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="20" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="1">
+      <c r="B20" s="5"/>
+      <c r="C20" s="1">
         <f>VLOOKUP(C$7,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.44</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D20" s="1">
         <f>VLOOKUP(D$7,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.07</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E20" s="1">
         <f>VLOOKUP(E$7,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F20" s="1">
         <f>VLOOKUP(F$7,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>0.92</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G20" s="1">
         <f>VLOOKUP(G$7,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.3</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H20" s="1">
         <f>VLOOKUP(C$8,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.92</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I20" s="1">
         <f>VLOOKUP(D$8,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.31</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J20" s="1">
         <f>VLOOKUP(E$8,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.1599999999999999</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K20" s="1">
         <f>VLOOKUP(F$8,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.06</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L20" s="1">
         <f>VLOOKUP(G$8,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.1399999999999999</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M20" s="1">
         <f>VLOOKUP(C$9,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="N17" s="1">
+      <c r="N20" s="1">
         <f>VLOOKUP(D$9,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>2.81</v>
       </c>
-      <c r="O17" s="1">
+      <c r="O20" s="1">
         <f>VLOOKUP(E$9,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.93</v>
       </c>
-      <c r="P17" s="1">
+      <c r="P20" s="1">
         <f>VLOOKUP(F$9,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.06</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="Q20" s="1">
         <f>VLOOKUP(G$9,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.53</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+    <row r="21" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="1">
+      <c r="B21" s="5"/>
+      <c r="C21" s="1">
         <f>VLOOKUP(C$10,Jobs!$J$2:'Jobs'!$K$31,2)</f>
         <v>1.67</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D21" s="1">
         <f>VLOOKUP(D$10,Jobs!$J$2:'Jobs'!$K$31,2)</f>
         <v>1.67</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E21" s="1">
         <f>VLOOKUP(E$10,Jobs!$J$2:'Jobs'!$K$31,2)</f>
         <v>1.67</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F21" s="1">
         <f>VLOOKUP(F$10,Jobs!$J$2:'Jobs'!$K$31,2)</f>
         <v>1.67</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G21" s="1">
         <f>VLOOKUP(G$10,Jobs!$J$2:'Jobs'!$K$31,2)</f>
         <v>1.67</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H21" s="1">
         <f>VLOOKUP(C$11,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>3.74</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I21" s="1">
         <f>VLOOKUP(D$11,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.86</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J21" s="1">
         <f>VLOOKUP(E$11,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>2.14</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K21" s="1">
         <f>VLOOKUP(F$11,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>3.57</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L21" s="1">
         <f>VLOOKUP(G$11,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>3.21</v>
       </c>
-      <c r="M18" s="1">
+      <c r="M21" s="1">
         <f>VLOOKUP(C$12,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>2.57</v>
       </c>
-      <c r="N18" s="1">
+      <c r="N21" s="1">
         <f>VLOOKUP(D$12,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>2.81</v>
       </c>
-      <c r="O18" s="1">
+      <c r="O21" s="1">
         <f>VLOOKUP(E$12,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>2.56</v>
       </c>
-      <c r="P18" s="1">
+      <c r="P21" s="1">
         <f>VLOOKUP(F$12,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>2.89</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="Q21" s="1">
         <f>VLOOKUP(G$12,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>1.99</v>
       </c>
-      <c r="R18" s="1">
+      <c r="R21" s="1">
         <f>VLOOKUP(C$13,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>2.4900000000000002</v>
       </c>
-      <c r="S18" s="1">
+      <c r="S21" s="1">
         <f>VLOOKUP(D$13,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>2.5</v>
       </c>
-      <c r="T18" s="1">
+      <c r="T21" s="1">
         <f>VLOOKUP(E$13,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>3.04</v>
       </c>
-      <c r="U18" s="1">
+      <c r="U21" s="1">
         <f>VLOOKUP(F$13,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>2.87</v>
       </c>
-      <c r="V18" s="1">
+      <c r="V21" s="1">
         <f>VLOOKUP(G$13,Jobs!$J$2:'Jobs'!$K$501,2)</f>
         <v>2.79</v>
       </c>
-      <c r="W18" s="1"/>
-    </row>
-    <row r="21" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="3" t="s">
+      <c r="W21" s="1"/>
+    </row>
+    <row r="24" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+    <row r="25" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="1">
-        <f>SUM(C16:L16)</f>
+      <c r="B25" s="5"/>
+      <c r="C25" s="1">
+        <f>SUM(C19:L19)</f>
         <v>5.58</v>
       </c>
-      <c r="D22" s="1">
-        <f>C22/Resources!B2</f>
+      <c r="D25" s="1">
+        <f>C25/Resources!B2</f>
         <v>5.58</v>
       </c>
-      <c r="E22" s="1">
-        <f>D22*Resources!C2</f>
+      <c r="E25" s="1">
+        <f>D25*Resources!C2</f>
         <v>5.5800000000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+    <row r="26" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="1">
-        <f>SUM(C17:Q17)</f>
+      <c r="B26" s="5"/>
+      <c r="C26" s="1">
+        <f>SUM(C20:Q20)</f>
         <v>20.86</v>
       </c>
-      <c r="D23" s="1">
-        <f>C23/Resources!B3</f>
+      <c r="D26" s="1">
+        <f>C26/Resources!B3</f>
         <v>10.43</v>
       </c>
-      <c r="E23" s="1">
-        <f>D23*Resources!C3</f>
+      <c r="E26" s="1">
+        <f>D26*Resources!C3</f>
         <v>0.20860000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+    <row r="27" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="1">
-        <f>SUM(C18:V18)</f>
+      <c r="B27" s="5"/>
+      <c r="C27" s="1">
+        <f>SUM(C21:V21)</f>
         <v>49.379999999999995</v>
       </c>
-      <c r="D24" s="1">
-        <f>C24/Resources!B4</f>
+      <c r="D27" s="1">
+        <f>C27/Resources!B4</f>
         <v>16.459999999999997</v>
       </c>
-      <c r="E24" s="1">
-        <f>D24*Resources!C4</f>
+      <c r="E27" s="1">
+        <f>D27*Resources!C4</f>
         <v>0.41149999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D26" t="s">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
         <v>15</v>
       </c>
-      <c r="E26">
-        <f>SUM(E22:E25)</f>
+      <c r="E29">
+        <f>SUM(E25:E28)</f>
         <v>0.67589999999999995</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G29" t="s">
         <v>18</v>
       </c>
-      <c r="H26">
+      <c r="H29">
         <v>0.8</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D27" t="s">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
         <v>16</v>
       </c>
-      <c r="E27">
-        <f>SUM(D22:D24)</f>
+      <c r="E30">
+        <f>SUM(D25:D27)</f>
         <v>32.47</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="D29" s="6" t="s">
+    <row r="32" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="D32" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7">
-        <f>E27</f>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7">
+        <f>E30</f>
         <v>32.47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="H17" formula="1"/>
+    <ignoredError sqref="H20" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update cell name to max time allowed
</commit_message>
<xml_diff>
--- a/cloud_scheduling.xlsx
+++ b/cloud_scheduling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\KE5207-FM-GA\CI2_GA_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A121C978-89C4-4E80-B321-EF3AE798B06E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{37912A06-A0D6-4CB6-BD9B-F0C749518F4F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,9 +193,6 @@
     <t>Max jobs allowed</t>
   </si>
   <si>
-    <t>Max cost allowed</t>
-  </si>
-  <si>
     <t>Current # jobs alloted</t>
   </si>
   <si>
@@ -209,6 +206,9 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>Max time allowed</t>
   </si>
 </sst>
 </file>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,7 +852,7 @@
         <v>20</v>
       </c>
       <c r="W1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X1" t="s">
         <v>6</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="14">
         <v>0</v>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="15">
         <v>0</v>
@@ -1450,10 +1450,10 @@
         <v>20</v>
       </c>
       <c r="Y12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="Z12">
-        <v>2.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
@@ -1532,10 +1532,10 @@
         <v>14</v>
       </c>
       <c r="AF14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AG14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
@@ -1610,7 +1610,7 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="AB18" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AC18" s="21">
         <v>4</v>
@@ -1630,7 +1630,7 @@
     </row>
     <row r="19" spans="5:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AB19" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC19" s="21">
         <v>5</v>

</xml_diff>

<commit_message>
Changed objective function and max time allowed
</commit_message>
<xml_diff>
--- a/cloud_scheduling.xlsx
+++ b/cloud_scheduling.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\KE5207-FM-GA\CI2_GA_code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MTechKE\Semester 2\computational intelligence ii\Lecture Notes\Day 1 and 2 (Fangming)\CA Git Code\genetic_algorithm_cloud_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{37912A06-A0D6-4CB6-BD9B-F0C749518F4F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="38400" windowHeight="23532"/>
   </bookViews>
   <sheets>
     <sheet name="Scheduling resources" sheetId="4" r:id="rId1"/>
@@ -25,10 +24,12 @@
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Scheduling resources'!$C$2:$V$6</definedName>
     <definedName name="solver_lhs10" localSheetId="0" hidden="1">'Scheduling resources'!$W$7</definedName>
     <definedName name="solver_lhs11" localSheetId="0" hidden="1">'Scheduling resources'!$W$7</definedName>
-    <definedName name="solver_lhs12" localSheetId="0" hidden="1">'Scheduling resources'!$Z$8</definedName>
+    <definedName name="solver_lhs12" localSheetId="0" hidden="1">'Scheduling resources'!$Z$9</definedName>
+    <definedName name="solver_lhs13" localSheetId="0" hidden="1">'Scheduling resources'!$Z$9</definedName>
+    <definedName name="solver_lhs14" localSheetId="0" hidden="1">'Scheduling resources'!$Z$9</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Scheduling resources'!$C$2:$V$6</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Scheduling resources'!$C$2:$V$6</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Scheduling resources'!$C$7:$L$7</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Scheduling resources'!$C$7:$V$7</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Scheduling resources'!$W$2</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Scheduling resources'!$W$3</definedName>
     <definedName name="solver_lhs7" localSheetId="0" hidden="1">'Scheduling resources'!$W$4</definedName>
@@ -42,13 +43,15 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">12</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Scheduling resources'!$Z$9</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Scheduling resources'!$Z$8</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel10" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel11" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel12" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel13" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel14" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
@@ -61,6 +64,8 @@
     <definedName name="solver_rhs10" localSheetId="0" hidden="1">'Scheduling resources'!$AD$21</definedName>
     <definedName name="solver_rhs11" localSheetId="0" hidden="1">'Scheduling resources'!$Z$11</definedName>
     <definedName name="solver_rhs12" localSheetId="0" hidden="1">'Scheduling resources'!$Z$12</definedName>
+    <definedName name="solver_rhs13" localSheetId="0" hidden="1">'Scheduling resources'!$Z$12</definedName>
+    <definedName name="solver_rhs14" localSheetId="0" hidden="1">'Scheduling resources'!$Z$12</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">integer</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">1</definedName>
@@ -80,17 +85,17 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="179017" calcMode="manual"/>
+  <calcPr calcId="162913" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Anurag Chatterjee</author>
   </authors>
   <commentList>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="Y1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -114,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="AF14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -143,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>A</t>
   </si>
@@ -209,12 +214,15 @@
   </si>
   <si>
     <t>Max time allowed</t>
+  </si>
+  <si>
+    <t>total time less than max time allowed constraint not applied</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -435,6 +443,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,23 +537,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -580,23 +572,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -772,22 +747,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AG21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="23" max="23" width="17.28515625" customWidth="1"/>
-    <col min="24" max="24" width="18.42578125" customWidth="1"/>
-    <col min="25" max="25" width="17.5703125" customWidth="1"/>
-    <col min="30" max="30" width="15.28515625" customWidth="1"/>
+    <col min="23" max="23" width="17.33203125" customWidth="1"/>
+    <col min="24" max="24" width="18.44140625" customWidth="1"/>
+    <col min="25" max="25" width="17.5546875" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -864,12 +839,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="6">
         <v>0</v>
@@ -902,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="N2" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="11">
         <v>0</v>
@@ -920,7 +895,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2" s="11">
         <v>0</v>
@@ -930,22 +905,22 @@
       </c>
       <c r="W2">
         <f>SUM(C2:V2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X2">
         <f>SUMPRODUCT(C2:V2,B13:U13)</f>
-        <v>0.15</v>
+        <v>2.6</v>
       </c>
       <c r="Y2">
         <f>X2/AC15</f>
-        <v>0.15</v>
+        <v>2.6</v>
       </c>
       <c r="Z2">
         <f>Y2*AD15</f>
-        <v>2.2499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -959,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="8">
         <v>0</v>
@@ -974,7 +949,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="8">
         <v>0</v>
@@ -983,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="1">
         <v>0</v>
@@ -1001,32 +976,32 @@
         <v>0</v>
       </c>
       <c r="T3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3" s="1">
         <v>0</v>
       </c>
       <c r="V3" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
         <f>SUM(C3:V3)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X3">
         <f>SUMPRODUCT(C3:V3,B13:U13)</f>
-        <v>1.28</v>
+        <v>3.04</v>
       </c>
       <c r="Y3">
         <f>X3/AC16</f>
-        <v>0.64</v>
+        <v>1.52</v>
       </c>
       <c r="Z3">
         <f>Y3*AD16</f>
-        <v>0.192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+        <v>0.45599999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1052,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="8">
         <v>0</v>
@@ -1067,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="1">
         <v>1</v>
@@ -1079,10 +1054,10 @@
         <v>1</v>
       </c>
       <c r="S4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="1">
         <v>0</v>
@@ -1096,18 +1071,18 @@
       </c>
       <c r="X4">
         <f>SUMPRODUCT(C4:V4,B13:U13)</f>
-        <v>3.9099999999999997</v>
+        <v>5.9700000000000006</v>
       </c>
       <c r="Y4">
         <f>X4/AC17</f>
-        <v>1.3033333333333332</v>
+        <v>1.9900000000000002</v>
       </c>
       <c r="Z4">
         <f>Y4*AD17</f>
-        <v>0.58650000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+        <v>0.89550000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -1124,19 +1099,19 @@
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>
       </c>
       <c r="K5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
@@ -1145,25 +1120,25 @@
         <v>0</v>
       </c>
       <c r="N5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" s="1">
         <v>0</v>
       </c>
       <c r="P5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="1">
         <v>0</v>
       </c>
       <c r="R5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" s="1">
         <v>1</v>
       </c>
       <c r="T5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5" s="1">
         <v>0</v>
@@ -1173,22 +1148,22 @@
       </c>
       <c r="W5">
         <f>SUM(C5:V5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X5">
         <f>SUMPRODUCT(C5:V5,B13:U13)</f>
-        <v>3.9099999999999997</v>
+        <v>5.7299999999999995</v>
       </c>
       <c r="Y5">
         <f>X5/AC18</f>
-        <v>0.97749999999999992</v>
+        <v>1.4324999999999999</v>
       </c>
       <c r="Z5">
         <f>Y5*AD18</f>
-        <v>0.48874999999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+        <v>1.4324999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -1196,46 +1171,46 @@
         <v>0</v>
       </c>
       <c r="D6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="16">
         <v>1</v>
       </c>
       <c r="F6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="16">
         <v>0</v>
       </c>
       <c r="H6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="16">
         <v>0</v>
       </c>
       <c r="J6" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="16">
         <v>0</v>
       </c>
       <c r="L6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6" s="16">
         <v>0</v>
       </c>
       <c r="P6" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" s="16">
         <v>0</v>
@@ -1244,39 +1219,39 @@
         <v>0</v>
       </c>
       <c r="T6" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" s="17">
         <v>0</v>
       </c>
       <c r="W6">
         <f>SUM(C6:V6)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="X6">
         <f>SUMPRODUCT(C6:V6,B13:U13)</f>
-        <v>3.3799999999999994</v>
+        <v>13.38</v>
       </c>
       <c r="Y6">
         <f>X6/AC18</f>
-        <v>0.84499999999999986</v>
+        <v>3.3450000000000002</v>
       </c>
       <c r="Z6">
         <f t="shared" ref="Z6" si="0">Y6*AD19</f>
-        <v>0.46474999999999994</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+        <v>5.0175000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="C7">
         <f t="shared" ref="C7:H7" si="1">SUM(C2:C6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
@@ -1288,96 +1263,96 @@
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7" si="2">SUM(I2:I4)</f>
-        <v>0</v>
+        <f>SUM(I2:I6)</f>
+        <v>1</v>
       </c>
       <c r="J7">
-        <f t="shared" ref="J7:X7" si="3">SUM(J2:J6)</f>
+        <f t="shared" ref="J7:X7" si="2">SUM(J2:J6)</f>
         <v>1</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="M7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="N7">
-        <f t="shared" si="3"/>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="O7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="P7">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="R7">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="S7">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="T7">
-        <f t="shared" si="3"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="U7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="V7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="W7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="X7">
-        <f t="shared" si="3"/>
-        <v>12.629999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>30.72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Y8" t="s">
         <v>9</v>
       </c>
-      <c r="Z8">
+      <c r="Z8" s="9">
         <f>SUM(Z2:Z6)</f>
-        <v>1.7544999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+        <v>8.1914999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Y9" t="s">
         <v>10</v>
       </c>
-      <c r="Z9" s="9">
+      <c r="Z9" s="22">
         <f>SUM(Y2:Y6)+INT(W2/AG15)*AF15+INT(W3/AG16)*AF16+INT(W4/AG17)*AF17+INT(W5/AG18)*AF18+INT(W6/AG19)*AF19</f>
-        <v>5.315833333333333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+        <v>12.387500000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Y11" t="s">
         <v>12</v>
       </c>
@@ -1385,7 +1360,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1453,10 +1428,10 @@
         <v>21</v>
       </c>
       <c r="Z12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1521,7 +1496,7 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="AC14" t="s">
         <v>2</v>
       </c>
@@ -1538,7 +1513,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="AB15" t="s">
         <v>0</v>
       </c>
@@ -1558,7 +1533,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <f>SUM(B13:U13)</f>
+        <v>30.72</v>
+      </c>
       <c r="AB16" t="s">
         <v>1</v>
       </c>
@@ -1578,7 +1557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="5:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:33" x14ac:dyDescent="0.3">
       <c r="AB17" t="s">
         <v>3</v>
       </c>
@@ -1598,7 +1577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="5:33" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:33" ht="16.2" x14ac:dyDescent="0.3">
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -1616,7 +1595,7 @@
         <v>4</v>
       </c>
       <c r="AD18" s="18">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AE18" s="19">
         <v>6</v>
@@ -1628,7 +1607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="5:33" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="AB19" s="8" t="s">
         <v>20</v>
       </c>
@@ -1636,10 +1615,10 @@
         <v>5</v>
       </c>
       <c r="AD19" s="20">
-        <v>0.55000000000000004</v>
+        <v>1.5</v>
       </c>
       <c r="AE19" s="19">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AF19" s="4">
         <v>0.3</v>
@@ -1648,13 +1627,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="5:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:33" x14ac:dyDescent="0.3">
       <c r="AC21" t="s">
         <v>15</v>
       </c>
       <c r="AD21">
         <f>SUM(AE15:AE19)</f>
-        <v>27</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="5:33" x14ac:dyDescent="0.3">
+      <c r="R22" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with premium server worksheet
</commit_message>
<xml_diff>
--- a/cloud_scheduling.xlsx
+++ b/cloud_scheduling.xlsx
@@ -1,93 +1,171 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierlim/PycharmProjects/genetic_algorithm_cloud_scheduling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierl\PycharmProjects\GA_cloud_schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171AE6A7-64D5-344A-BAC0-A04F7800D10E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0815E4-4FDE-4EDF-ADAD-736B4A817BD5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="456" windowWidth="19200" windowHeight="23544" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scheduling resources" sheetId="4" r:id="rId1"/>
+    <sheet name="Testing Premium Servers Pricing" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Scheduling resources'!$C$2:$V$6</definedName>
-    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.00001</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$C$2:$V$6</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Scheduling resources'!$C$2:$V$6</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$C$2:$V$6</definedName>
     <definedName name="solver_lhs10" localSheetId="0" hidden="1">'Scheduling resources'!$W$7</definedName>
+    <definedName name="solver_lhs10" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$7</definedName>
     <definedName name="solver_lhs11" localSheetId="0" hidden="1">'Scheduling resources'!$W$7</definedName>
+    <definedName name="solver_lhs11" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$7</definedName>
     <definedName name="solver_lhs12" localSheetId="0" hidden="1">'Scheduling resources'!$Z$9</definedName>
+    <definedName name="solver_lhs12" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$9</definedName>
     <definedName name="solver_lhs13" localSheetId="0" hidden="1">'Scheduling resources'!$Z$9</definedName>
+    <definedName name="solver_lhs13" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$9</definedName>
     <definedName name="solver_lhs14" localSheetId="0" hidden="1">'Scheduling resources'!$Z$9</definedName>
+    <definedName name="solver_lhs14" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$9</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Scheduling resources'!$C$2:$V$6</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$C$2:$V$6</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Scheduling resources'!$C$2:$V$6</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$C$2:$V$6</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Scheduling resources'!$C$7:$V$7</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$C$7:$V$7</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Scheduling resources'!$W$2</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$2</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Scheduling resources'!$W$3</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$3</definedName>
     <definedName name="solver_lhs7" localSheetId="0" hidden="1">'Scheduling resources'!$W$4</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$4</definedName>
     <definedName name="solver_lhs8" localSheetId="0" hidden="1">'Scheduling resources'!$W$5</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$5</definedName>
     <definedName name="solver_lhs9" localSheetId="0" hidden="1">'Scheduling resources'!$W$6</definedName>
+    <definedName name="solver_lhs9" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$6</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">60</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">60</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.001</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.001</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">12</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">12</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Scheduling resources'!$Z$8</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$8</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel10" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel10" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel11" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel11" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel12" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel12" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel13" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel13" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel14" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel14" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">4</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel7" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel8" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel9" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs10" localSheetId="0" hidden="1">'Scheduling resources'!$AD$21</definedName>
+    <definedName name="solver_rhs10" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$AD$21</definedName>
     <definedName name="solver_rhs11" localSheetId="0" hidden="1">'Scheduling resources'!$Z$11</definedName>
+    <definedName name="solver_rhs11" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$11</definedName>
     <definedName name="solver_rhs12" localSheetId="0" hidden="1">'Scheduling resources'!$Z$12</definedName>
+    <definedName name="solver_rhs12" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$12</definedName>
     <definedName name="solver_rhs13" localSheetId="0" hidden="1">'Scheduling resources'!$Z$12</definedName>
+    <definedName name="solver_rhs13" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$12</definedName>
     <definedName name="solver_rhs14" localSheetId="0" hidden="1">'Scheduling resources'!$Z$12</definedName>
+    <definedName name="solver_rhs14" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$12</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">integer</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">integer</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">'Scheduling resources'!$AE$15</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$AE$15</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">'Scheduling resources'!$AE$16</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$AE$16</definedName>
     <definedName name="solver_rhs7" localSheetId="0" hidden="1">'Scheduling resources'!$AE$17</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$AE$17</definedName>
     <definedName name="solver_rhs8" localSheetId="0" hidden="1">'Scheduling resources'!$AE$18</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$AE$18</definedName>
     <definedName name="solver_rhs9" localSheetId="0" hidden="1">'Scheduling resources'!$AE$19</definedName>
+    <definedName name="solver_rhs9" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$AE$19</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">1000</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">1000</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -149,8 +227,66 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Anurag Chatterjee</author>
+  </authors>
+  <commentList>
+    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{0610CA40-74CC-4C6A-88A9-423C5F9D4B31}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anurag Chatterjee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Calculated by dividing by efficiency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AF14" authorId="0" shapeId="0" xr:uid="{4AD4F2B4-667F-47B7-B100-1FB01AA12979}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anurag Chatterjee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+After pre-emtion # jobs the machine is unavailable for pre emption time and so it adds to the time</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
   <si>
     <t>A</t>
   </si>
@@ -217,6 +353,21 @@
   <si>
     <t>Max time allowed</t>
   </si>
+  <si>
+    <t>Premium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premium </t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>Server Class</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
 </sst>
 </file>
 
@@ -279,7 +430,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -411,11 +562,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -443,6 +609,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,19 +958,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="130" workbookViewId="0">
-      <selection activeCell="X29" sqref="X29"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
+      <selection activeCell="Z8" sqref="B1:Z9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="23" max="23" width="17.33203125" customWidth="1"/>
-    <col min="24" max="24" width="18.5" customWidth="1"/>
-    <col min="25" max="25" width="17.5" customWidth="1"/>
+    <col min="24" max="24" width="18.44140625" customWidth="1"/>
+    <col min="25" max="25" width="17.44140625" customWidth="1"/>
     <col min="30" max="30" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -872,15 +1047,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="6">
         <v>0</v>
@@ -892,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="6">
         <v>0</v>
@@ -913,58 +1088,58 @@
         <v>0</v>
       </c>
       <c r="O2" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" s="11">
         <v>0</v>
       </c>
       <c r="Q2" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2" s="11">
         <v>0</v>
       </c>
       <c r="T2" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2" s="11">
         <v>0</v>
       </c>
       <c r="V2" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2">
         <f>SUM(C2:V2)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X2">
         <f>SUMPRODUCT(C2:V2,B13:U13)</f>
-        <v>3.9099999999999997</v>
+        <v>11.71</v>
       </c>
       <c r="Y2">
         <f>X2/AC15</f>
-        <v>3.9099999999999997</v>
+        <v>11.71</v>
       </c>
       <c r="Z2">
         <f>Y2*AD15</f>
-        <v>0.58649999999999991</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+        <v>1.7565000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
       </c>
       <c r="E3" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="8">
         <v>0</v>
@@ -973,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="8">
         <v>0</v>
@@ -985,10 +1160,10 @@
         <v>0</v>
       </c>
       <c r="L3" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="1">
         <v>0</v>
@@ -1006,7 +1181,7 @@
         <v>0</v>
       </c>
       <c r="S3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" s="1">
         <v>0</v>
@@ -1015,26 +1190,26 @@
         <v>0</v>
       </c>
       <c r="V3" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3">
         <f>SUM(C3:V3)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X3">
         <f>SUMPRODUCT(C3:V3,B13:U13)</f>
-        <v>3.79</v>
+        <v>9.18</v>
       </c>
       <c r="Y3">
         <f>X3/AC16</f>
-        <v>1.895</v>
+        <v>4.59</v>
       </c>
       <c r="Z3">
         <f>Y3*AD16</f>
-        <v>0.56850000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+        <v>1.377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1048,19 +1223,19 @@
         <v>0</v>
       </c>
       <c r="F4" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="8">
         <v>0</v>
       </c>
       <c r="I4" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="8">
         <v>0</v>
@@ -1072,10 +1247,10 @@
         <v>0</v>
       </c>
       <c r="N4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="1">
         <v>1</v>
@@ -1084,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="R4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="1">
         <v>0</v>
@@ -1093,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="U4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4" s="13">
         <v>0</v>
@@ -1104,18 +1279,18 @@
       </c>
       <c r="X4">
         <f>SUMPRODUCT(C4:V4,B13:U13)</f>
-        <v>5.9700000000000006</v>
+        <v>7.3000000000000007</v>
       </c>
       <c r="Y4">
         <f>X4/AC17</f>
-        <v>1.9900000000000002</v>
+        <v>2.4333333333333336</v>
       </c>
       <c r="Z4">
         <f>Y4*AD17</f>
-        <v>0.89550000000000007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+        <v>1.0950000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -1132,16 +1307,16 @@
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1">
         <v>1</v>
@@ -1150,10 +1325,10 @@
         <v>0</v>
       </c>
       <c r="M5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" s="1">
         <v>0</v>
@@ -1168,10 +1343,10 @@
         <v>0</v>
       </c>
       <c r="S5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5" s="1">
         <v>0</v>
@@ -1181,22 +1356,22 @@
       </c>
       <c r="W5">
         <f>SUM(C5:V5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X5">
         <f>SUMPRODUCT(C5:V5,B13:U13)</f>
-        <v>7.26</v>
+        <v>1.7799999999999998</v>
       </c>
       <c r="Y5">
         <f>X5/AC18</f>
-        <v>1.8149999999999999</v>
+        <v>0.44499999999999995</v>
       </c>
       <c r="Z5">
         <f>Y5*AD18</f>
-        <v>1.8149999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+        <v>0.44499999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -1204,13 +1379,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="16">
         <v>0</v>
@@ -1228,7 +1403,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="16">
         <v>0</v>
@@ -1243,7 +1418,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6" s="16">
         <v>0</v>
@@ -1255,29 +1430,29 @@
         <v>0</v>
       </c>
       <c r="U6" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6" s="17">
         <v>0</v>
       </c>
       <c r="W6">
         <f>SUM(C6:V6)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="X6">
         <f>SUMPRODUCT(C6:V6,B13:U13)</f>
-        <v>9.7900000000000009</v>
+        <v>0.75</v>
       </c>
       <c r="Y6">
         <f>X6/AC18</f>
-        <v>2.4475000000000002</v>
+        <v>0.1875</v>
       </c>
       <c r="Z6">
         <f t="shared" ref="Z6" si="0">Y6*AD19</f>
-        <v>3.6712500000000006</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+        <v>0.28125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="C7">
         <f t="shared" ref="C7:H7" si="1">SUM(C2:C6)</f>
         <v>1</v>
@@ -1364,28 +1539,28 @@
       </c>
       <c r="X7">
         <f t="shared" si="2"/>
-        <v>30.72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+        <v>30.720000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Y8" t="s">
         <v>9</v>
       </c>
       <c r="Z8" s="9">
         <f>SUM(Z2:Z6)</f>
-        <v>7.5367500000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+        <v>4.9547500000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Y9" t="s">
         <v>10</v>
       </c>
       <c r="Z9" s="22">
         <f>SUM(Y2:Y6)+INT(W2/AG15)*AF15+INT(W3/AG16)*AF16+INT(W4/AG17)*AF17+INT(W5/AG18)*AF18+INT(W6/AG19)*AF19</f>
-        <v>13.2575</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+        <v>20.565833333333334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Y11" t="s">
         <v>12</v>
       </c>
@@ -1393,7 +1568,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1461,10 +1636,10 @@
         <v>21</v>
       </c>
       <c r="Z12">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1529,7 +1704,7 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="AC14" t="s">
         <v>2</v>
       </c>
@@ -1546,7 +1721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="AB15" t="s">
         <v>0</v>
       </c>
@@ -1566,7 +1741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="G16">
         <f>SUM(B13:U13)</f>
         <v>30.72</v>
@@ -1590,7 +1765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="5:33" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:33" x14ac:dyDescent="0.3">
       <c r="AB17" t="s">
         <v>3</v>
       </c>
@@ -1610,7 +1785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="5:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:33" ht="16.2" x14ac:dyDescent="0.3">
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -1640,7 +1815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="5:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="AB19" s="8" t="s">
         <v>20</v>
       </c>
@@ -1660,7 +1835,928 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="5:33" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:33" x14ac:dyDescent="0.3">
+      <c r="AC21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD21">
+        <f>SUM(AE15:AE19)</f>
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CEA69A-D98C-4A31-9599-286FAD3E94CA}">
+  <dimension ref="A1:AG21"/>
+  <sheetViews>
+    <sheetView zoomScale="130" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="23" max="23" width="17.33203125" customWidth="1"/>
+    <col min="24" max="24" width="18.44140625" customWidth="1"/>
+    <col min="25" max="25" width="17.44140625" customWidth="1"/>
+    <col min="27" max="27" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.88671875" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" customWidth="1"/>
+    <col min="32" max="32" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="11">
+        <v>0</v>
+      </c>
+      <c r="N2" s="11">
+        <v>0</v>
+      </c>
+      <c r="O2" s="11">
+        <v>0</v>
+      </c>
+      <c r="P2" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>1</v>
+      </c>
+      <c r="R2" s="11">
+        <v>0</v>
+      </c>
+      <c r="S2" s="11">
+        <v>0</v>
+      </c>
+      <c r="T2" s="11">
+        <v>0</v>
+      </c>
+      <c r="U2" s="11">
+        <v>0</v>
+      </c>
+      <c r="V2" s="12">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <f>SUM(C2:V2)</f>
+        <v>3</v>
+      </c>
+      <c r="X2">
+        <f>SUMPRODUCT(C2:V2,B13:U13)</f>
+        <v>6.78</v>
+      </c>
+      <c r="Y2">
+        <f>X2/AC15</f>
+        <v>6.78</v>
+      </c>
+      <c r="Z2">
+        <f>Y2*AD15</f>
+        <v>1.0169999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="13">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <f>SUM(C3:V3)</f>
+        <v>5</v>
+      </c>
+      <c r="X3">
+        <f>SUMPRODUCT(C3:V3,B13:U13)</f>
+        <v>10.609999999999998</v>
+      </c>
+      <c r="Y3">
+        <f>X3/AC16</f>
+        <v>5.3049999999999988</v>
+      </c>
+      <c r="Z3">
+        <f>Y3*AD16</f>
+        <v>1.5914999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8">
+        <v>1</v>
+      </c>
+      <c r="L4" s="8">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="V4" s="13">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <f>SUM(C4:V4)</f>
+        <v>4</v>
+      </c>
+      <c r="X4">
+        <f>SUMPRODUCT(C4:V4,B13:U13)</f>
+        <v>5.09</v>
+      </c>
+      <c r="Y4">
+        <f>X4/AC17</f>
+        <v>1.6966666666666665</v>
+      </c>
+      <c r="Z4">
+        <f>Y4*AD17</f>
+        <v>0.76349999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1">
+        <v>1</v>
+      </c>
+      <c r="V5" s="13">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <f>SUM(C5:V5)</f>
+        <v>5</v>
+      </c>
+      <c r="X5">
+        <f>SUMPRODUCT(C5:V5,B13:U13)</f>
+        <v>3.6799999999999997</v>
+      </c>
+      <c r="Y5">
+        <f>X5/AC18</f>
+        <v>0.91999999999999993</v>
+      </c>
+      <c r="Z5">
+        <f>Y5*AD18</f>
+        <v>1.8399999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
+        <v>1</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16">
+        <v>0</v>
+      </c>
+      <c r="I6" s="16">
+        <v>0</v>
+      </c>
+      <c r="J6" s="16">
+        <v>1</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0</v>
+      </c>
+      <c r="L6" s="16">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <v>0</v>
+      </c>
+      <c r="O6" s="16">
+        <v>1</v>
+      </c>
+      <c r="P6" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="16">
+        <v>0</v>
+      </c>
+      <c r="R6" s="16">
+        <v>0</v>
+      </c>
+      <c r="S6" s="16">
+        <v>0</v>
+      </c>
+      <c r="T6" s="16">
+        <v>0</v>
+      </c>
+      <c r="U6" s="16">
+        <v>0</v>
+      </c>
+      <c r="V6" s="17">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <f>SUM(C6:V6)</f>
+        <v>3</v>
+      </c>
+      <c r="X6">
+        <f>SUMPRODUCT(C6:V6,B13:U13)</f>
+        <v>4.5600000000000005</v>
+      </c>
+      <c r="Y6">
+        <f>X6/AC18</f>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" ref="Z6" si="0">Y6*AD19</f>
+        <v>5.7000000000000011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f t="shared" ref="C7:H7" si="1">SUM(C2:C6)</f>
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f>SUM(I2:I6)</f>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7:X7" si="2">SUM(J2:J6)</f>
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="2"/>
+        <v>30.72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Y8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="9">
+        <f>SUM(Z2:Z6)</f>
+        <v>10.912000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Y9" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z9" s="22">
+        <f>SUM(Y2:Y6)+INT(W2/AG15)*AF15+INT(W3/AG16)*AF16+INT(W4/AG17)*AF17+INT(W5/AG18)*AF18+INT(W6/AG19)*AF19</f>
+        <v>17.241666666666667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Y11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="23">
+        <v>1</v>
+      </c>
+      <c r="C12" s="23">
+        <v>2</v>
+      </c>
+      <c r="D12" s="23">
+        <v>3</v>
+      </c>
+      <c r="E12" s="23">
+        <v>4</v>
+      </c>
+      <c r="F12" s="23">
+        <v>5</v>
+      </c>
+      <c r="G12" s="23">
+        <v>6</v>
+      </c>
+      <c r="H12" s="23">
+        <v>7</v>
+      </c>
+      <c r="I12" s="23">
+        <v>8</v>
+      </c>
+      <c r="J12" s="23">
+        <v>9</v>
+      </c>
+      <c r="K12" s="23">
+        <v>10</v>
+      </c>
+      <c r="L12" s="23">
+        <v>11</v>
+      </c>
+      <c r="M12" s="23">
+        <v>12</v>
+      </c>
+      <c r="N12" s="23">
+        <v>13</v>
+      </c>
+      <c r="O12" s="23">
+        <v>14</v>
+      </c>
+      <c r="P12" s="23">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="23">
+        <v>16</v>
+      </c>
+      <c r="R12" s="23">
+        <v>17</v>
+      </c>
+      <c r="S12" s="23">
+        <v>18</v>
+      </c>
+      <c r="T12" s="23">
+        <v>19</v>
+      </c>
+      <c r="U12" s="23">
+        <v>20</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="23">
+        <v>1.99</v>
+      </c>
+      <c r="C13" s="23">
+        <v>1.93</v>
+      </c>
+      <c r="D13" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="E13" s="23">
+        <v>0.42</v>
+      </c>
+      <c r="F13" s="23">
+        <v>2.57</v>
+      </c>
+      <c r="G13" s="23">
+        <v>1.31</v>
+      </c>
+      <c r="H13" s="23">
+        <v>1.92</v>
+      </c>
+      <c r="I13" s="23">
+        <v>0.92</v>
+      </c>
+      <c r="J13" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="K13" s="23">
+        <v>3.21</v>
+      </c>
+      <c r="L13" s="23">
+        <v>1.53</v>
+      </c>
+      <c r="M13" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="N13" s="23">
+        <v>2.89</v>
+      </c>
+      <c r="O13" s="23">
+        <v>0.95</v>
+      </c>
+      <c r="P13" s="23">
+        <v>2.79</v>
+      </c>
+      <c r="Q13" s="23">
+        <v>1.06</v>
+      </c>
+      <c r="R13" s="23">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="S13" s="23">
+        <v>0.61</v>
+      </c>
+      <c r="T13" s="23">
+        <v>1.44</v>
+      </c>
+      <c r="U13" s="23">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AA14" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB14" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC14" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD14" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE14" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF14" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG14" s="23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AA15" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB15" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="24">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="AE15" s="24">
+        <v>5</v>
+      </c>
+      <c r="AF15" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="AG15" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <f>SUM(B13:U13)</f>
+        <v>30.72</v>
+      </c>
+      <c r="AA16" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB16" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="24">
+        <v>2</v>
+      </c>
+      <c r="AD16" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="AE16" s="24">
+        <v>5</v>
+      </c>
+      <c r="AF16" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="AG16" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="5:33" x14ac:dyDescent="0.3">
+      <c r="AA17" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB17" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC17" s="24">
+        <v>3</v>
+      </c>
+      <c r="AD17" s="24">
+        <v>0.45</v>
+      </c>
+      <c r="AE17" s="24">
+        <v>5</v>
+      </c>
+      <c r="AF17" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="AG17" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="5:33" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="AA18" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB18" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC18" s="25">
+        <v>4</v>
+      </c>
+      <c r="AD18" s="26">
+        <v>2</v>
+      </c>
+      <c r="AE18" s="25">
+        <v>6</v>
+      </c>
+      <c r="AF18" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="AG18" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="5:33" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AA19" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB19" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC19" s="25">
+        <v>5</v>
+      </c>
+      <c r="AD19" s="27">
+        <v>5</v>
+      </c>
+      <c r="AE19" s="25">
+        <v>10</v>
+      </c>
+      <c r="AF19" s="25">
+        <v>0.3</v>
+      </c>
+      <c r="AG19" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="5:33" x14ac:dyDescent="0.3">
       <c r="AC21" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Changed the max time allowed
</commit_message>
<xml_diff>
--- a/cloud_scheduling.xlsx
+++ b/cloud_scheduling.xlsx
@@ -1,164 +1,234 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierl\PycharmProjects\GA_cloud_schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MTechKE\Semester 2\computational intelligence ii\Lecture Notes\Day 1 and 2 (Fangming)\CA Git Code\genetic_algorithm_cloud_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0815E4-4FDE-4EDF-ADAD-736B4A817BD5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="456" windowWidth="19200" windowHeight="23544" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="456" windowWidth="19200" windowHeight="23544" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Scheduling resources" sheetId="4" r:id="rId1"/>
-    <sheet name="Testing Premium Servers Pricing" sheetId="5" r:id="rId2"/>
+    <sheet name="Scenario1-Less Time for jobs" sheetId="4" r:id="rId1"/>
+    <sheet name="Scenario2-More Time for job " sheetId="7" r:id="rId2"/>
+    <sheet name="Scenario3-Pricing Strategy" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Scheduling resources'!$C$2:$V$6</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$C$2:$V$6</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$C$2:$V$6</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$C$2:$V$6</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$C$2:$V$6</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Scheduling resources'!$C$2:$V$6</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$C$2:$V$6</definedName>
-    <definedName name="solver_lhs10" localSheetId="0" hidden="1">'Scheduling resources'!$W$7</definedName>
-    <definedName name="solver_lhs10" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$7</definedName>
-    <definedName name="solver_lhs11" localSheetId="0" hidden="1">'Scheduling resources'!$W$7</definedName>
-    <definedName name="solver_lhs11" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$7</definedName>
-    <definedName name="solver_lhs12" localSheetId="0" hidden="1">'Scheduling resources'!$Z$9</definedName>
-    <definedName name="solver_lhs12" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$9</definedName>
-    <definedName name="solver_lhs13" localSheetId="0" hidden="1">'Scheduling resources'!$Z$9</definedName>
-    <definedName name="solver_lhs13" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$9</definedName>
-    <definedName name="solver_lhs14" localSheetId="0" hidden="1">'Scheduling resources'!$Z$9</definedName>
-    <definedName name="solver_lhs14" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$9</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Scheduling resources'!$C$2:$V$6</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$C$2:$V$6</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Scheduling resources'!$C$2:$V$6</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$C$2:$V$6</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Scheduling resources'!$C$7:$V$7</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$C$7:$V$7</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Scheduling resources'!$W$2</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$2</definedName>
-    <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Scheduling resources'!$W$3</definedName>
-    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$3</definedName>
-    <definedName name="solver_lhs7" localSheetId="0" hidden="1">'Scheduling resources'!$W$4</definedName>
-    <definedName name="solver_lhs7" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$4</definedName>
-    <definedName name="solver_lhs8" localSheetId="0" hidden="1">'Scheduling resources'!$W$5</definedName>
-    <definedName name="solver_lhs8" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$5</definedName>
-    <definedName name="solver_lhs9" localSheetId="0" hidden="1">'Scheduling resources'!$W$6</definedName>
-    <definedName name="solver_lhs9" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$W$6</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$C$2:$V$6</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$C$2:$V$6</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$C$2:$V$6</definedName>
+    <definedName name="solver_lhs10" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$W$7</definedName>
+    <definedName name="solver_lhs10" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$W$7</definedName>
+    <definedName name="solver_lhs10" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$W$7</definedName>
+    <definedName name="solver_lhs11" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$W$7</definedName>
+    <definedName name="solver_lhs11" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$W$7</definedName>
+    <definedName name="solver_lhs11" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$W$7</definedName>
+    <definedName name="solver_lhs12" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$Z$9</definedName>
+    <definedName name="solver_lhs12" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$Z$9</definedName>
+    <definedName name="solver_lhs12" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$Z$9</definedName>
+    <definedName name="solver_lhs13" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$Z$9</definedName>
+    <definedName name="solver_lhs13" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$Z$9</definedName>
+    <definedName name="solver_lhs13" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$Z$9</definedName>
+    <definedName name="solver_lhs14" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$Z$9</definedName>
+    <definedName name="solver_lhs14" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$Z$9</definedName>
+    <definedName name="solver_lhs14" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$Z$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$C$2:$V$6</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$C$2:$V$6</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$C$2:$V$6</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$C$2:$V$6</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$C$2:$V$6</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$C$2:$V$6</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$C$7:$V$7</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$C$7:$V$7</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$C$7:$V$7</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$W$2</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$W$2</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$W$2</definedName>
+    <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$W$3</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$W$3</definedName>
+    <definedName name="solver_lhs6" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$W$3</definedName>
+    <definedName name="solver_lhs7" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$W$4</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$W$4</definedName>
+    <definedName name="solver_lhs7" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$W$4</definedName>
+    <definedName name="solver_lhs8" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$W$5</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$W$5</definedName>
+    <definedName name="solver_lhs8" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$W$5</definedName>
+    <definedName name="solver_lhs9" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$W$6</definedName>
+    <definedName name="solver_lhs9" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$W$6</definedName>
+    <definedName name="solver_lhs9" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$W$6</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">60</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">60</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">60</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.001</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.001</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.001</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">12</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">12</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">12</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Scheduling resources'!$Z$8</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$8</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$Z$8</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$Z$8</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$Z$8</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel10" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel10" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel10" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel11" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel11" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel11" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel12" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel12" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel12" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel13" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel13" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel13" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel14" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel14" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel14" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">4</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">4</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel6" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel7" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel7" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel8" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel8" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel9" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel9" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rhs10" localSheetId="0" hidden="1">'Scheduling resources'!$AD$21</definedName>
-    <definedName name="solver_rhs10" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$AD$21</definedName>
-    <definedName name="solver_rhs11" localSheetId="0" hidden="1">'Scheduling resources'!$Z$11</definedName>
-    <definedName name="solver_rhs11" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$11</definedName>
-    <definedName name="solver_rhs12" localSheetId="0" hidden="1">'Scheduling resources'!$Z$12</definedName>
-    <definedName name="solver_rhs12" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$12</definedName>
-    <definedName name="solver_rhs13" localSheetId="0" hidden="1">'Scheduling resources'!$Z$12</definedName>
-    <definedName name="solver_rhs13" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$12</definedName>
-    <definedName name="solver_rhs14" localSheetId="0" hidden="1">'Scheduling resources'!$Z$12</definedName>
-    <definedName name="solver_rhs14" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$Z$12</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs10" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$AD$21</definedName>
+    <definedName name="solver_rhs10" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$AD$21</definedName>
+    <definedName name="solver_rhs10" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$AD$21</definedName>
+    <definedName name="solver_rhs11" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$Z$11</definedName>
+    <definedName name="solver_rhs11" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$Z$11</definedName>
+    <definedName name="solver_rhs11" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$Z$11</definedName>
+    <definedName name="solver_rhs12" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$Z$12</definedName>
+    <definedName name="solver_rhs12" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$Z$12</definedName>
+    <definedName name="solver_rhs12" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$Z$12</definedName>
+    <definedName name="solver_rhs13" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$Z$12</definedName>
+    <definedName name="solver_rhs13" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$Z$12</definedName>
+    <definedName name="solver_rhs13" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$Z$12</definedName>
+    <definedName name="solver_rhs14" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$Z$12</definedName>
+    <definedName name="solver_rhs14" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$Z$12</definedName>
+    <definedName name="solver_rhs14" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$Z$12</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">integer</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">integer</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">integer</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs4" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rhs5" localSheetId="0" hidden="1">'Scheduling resources'!$AE$15</definedName>
-    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$AE$15</definedName>
-    <definedName name="solver_rhs6" localSheetId="0" hidden="1">'Scheduling resources'!$AE$16</definedName>
-    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$AE$16</definedName>
-    <definedName name="solver_rhs7" localSheetId="0" hidden="1">'Scheduling resources'!$AE$17</definedName>
-    <definedName name="solver_rhs7" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$AE$17</definedName>
-    <definedName name="solver_rhs8" localSheetId="0" hidden="1">'Scheduling resources'!$AE$18</definedName>
-    <definedName name="solver_rhs8" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$AE$18</definedName>
-    <definedName name="solver_rhs9" localSheetId="0" hidden="1">'Scheduling resources'!$AE$19</definedName>
-    <definedName name="solver_rhs9" localSheetId="1" hidden="1">'Testing Premium Servers Pricing'!$AE$19</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$AE$15</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$AE$15</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$AE$15</definedName>
+    <definedName name="solver_rhs6" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$AE$16</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$AE$16</definedName>
+    <definedName name="solver_rhs6" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$AE$16</definedName>
+    <definedName name="solver_rhs7" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$AE$17</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$AE$17</definedName>
+    <definedName name="solver_rhs7" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$AE$17</definedName>
+    <definedName name="solver_rhs8" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$AE$18</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$AE$18</definedName>
+    <definedName name="solver_rhs8" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$AE$18</definedName>
+    <definedName name="solver_rhs9" localSheetId="0" hidden="1">'Scenario1-Less Time for jobs'!$AE$19</definedName>
+    <definedName name="solver_rhs9" localSheetId="1" hidden="1">'Scenario2-More Time for job '!$AE$19</definedName>
+    <definedName name="solver_rhs9" localSheetId="2" hidden="1">'Scenario3-Pricing Strategy'!$AE$19</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">1000</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">1000</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">1000</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -170,12 +240,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Anurag Chatterjee</author>
   </authors>
   <commentList>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="Y1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -199,7 +269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="AF14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -228,12 +298,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Anurag Chatterjee</author>
   </authors>
   <commentList>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{0610CA40-74CC-4C6A-88A9-423C5F9D4B31}">
+    <comment ref="Y1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -257,7 +327,65 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF14" authorId="0" shapeId="0" xr:uid="{4AD4F2B4-667F-47B7-B100-1FB01AA12979}">
+    <comment ref="AF14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anurag Chatterjee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+After pre-emtion # jobs the machine is unavailable for pre emption time and so it adds to the time</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Anurag Chatterjee</author>
+  </authors>
+  <commentList>
+    <comment ref="Y1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anurag Chatterjee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Calculated by dividing by efficiency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AF14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -286,7 +414,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="27">
   <si>
     <t>A</t>
   </si>
@@ -372,7 +500,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -711,23 +839,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -763,23 +874,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -955,11 +1049,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
-      <selection activeCell="Z8" sqref="B1:Z9"/>
+    <sheetView topLeftCell="J1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="6">
         <v>0</v>
@@ -1076,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="6">
         <v>0</v>
@@ -1088,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" s="11">
         <v>0</v>
@@ -1106,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="U2" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2" s="12">
         <v>1</v>
@@ -1117,15 +1211,15 @@
       </c>
       <c r="X2">
         <f>SUMPRODUCT(C2:V2,B13:U13)</f>
-        <v>11.71</v>
+        <v>8.43</v>
       </c>
       <c r="Y2">
         <f>X2/AC15</f>
-        <v>11.71</v>
+        <v>8.43</v>
       </c>
       <c r="Z2">
         <f>Y2*AD15</f>
-        <v>1.7565000000000002</v>
+        <v>1.2645</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
@@ -1145,7 +1239,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -1181,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="S3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3" s="1">
         <v>0</v>
@@ -1198,15 +1292,15 @@
       </c>
       <c r="X3">
         <f>SUMPRODUCT(C3:V3,B13:U13)</f>
-        <v>9.18</v>
+        <v>10.609999999999998</v>
       </c>
       <c r="Y3">
         <f>X3/AC16</f>
-        <v>4.59</v>
+        <v>5.3049999999999988</v>
       </c>
       <c r="Z3">
         <f>Y3*AD16</f>
-        <v>1.377</v>
+        <v>1.5914999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
@@ -1226,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="8">
         <v>0</v>
@@ -1247,13 +1341,13 @@
         <v>0</v>
       </c>
       <c r="N4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" s="1">
         <v>0</v>
       </c>
       <c r="P4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="1">
         <v>0</v>
@@ -1268,26 +1362,26 @@
         <v>0</v>
       </c>
       <c r="U4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="13">
         <v>0</v>
       </c>
       <c r="W4">
         <f>SUM(C4:V4)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X4">
         <f>SUMPRODUCT(C4:V4,B13:U13)</f>
-        <v>7.3000000000000007</v>
+        <v>2.4899999999999998</v>
       </c>
       <c r="Y4">
         <f>X4/AC17</f>
-        <v>2.4333333333333336</v>
+        <v>0.83</v>
       </c>
       <c r="Z4">
         <f>Y4*AD17</f>
-        <v>1.0950000000000002</v>
+        <v>0.3735</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -1298,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -1316,10 +1410,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
@@ -1328,13 +1422,13 @@
         <v>0</v>
       </c>
       <c r="N5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" s="1">
         <v>0</v>
       </c>
       <c r="P5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="1">
         <v>0</v>
@@ -1343,10 +1437,10 @@
         <v>0</v>
       </c>
       <c r="S5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5" s="1">
         <v>0</v>
@@ -1356,19 +1450,19 @@
       </c>
       <c r="W5">
         <f>SUM(C5:V5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X5">
         <f>SUMPRODUCT(C5:V5,B13:U13)</f>
-        <v>1.7799999999999998</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="Y5">
         <f>X5/AC18</f>
-        <v>0.44499999999999995</v>
+        <v>1.0049999999999999</v>
       </c>
       <c r="Z5">
         <f>Y5*AD18</f>
-        <v>0.44499999999999995</v>
+        <v>1.0049999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
@@ -1397,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="16">
         <v>0</v>
@@ -1412,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="O6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" s="16">
         <v>0</v>
@@ -1427,7 +1521,7 @@
         <v>0</v>
       </c>
       <c r="T6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" s="16">
         <v>0</v>
@@ -1437,19 +1531,19 @@
       </c>
       <c r="W6">
         <f>SUM(C6:V6)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="X6">
         <f>SUMPRODUCT(C6:V6,B13:U13)</f>
-        <v>0.75</v>
+        <v>5.1700000000000008</v>
       </c>
       <c r="Y6">
         <f>X6/AC18</f>
-        <v>0.1875</v>
+        <v>1.2925000000000002</v>
       </c>
       <c r="Z6">
         <f t="shared" ref="Z6" si="0">Y6*AD19</f>
-        <v>0.28125</v>
+        <v>1.9387500000000002</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
@@ -1539,7 +1633,7 @@
       </c>
       <c r="X7">
         <f t="shared" si="2"/>
-        <v>30.720000000000002</v>
+        <v>30.72</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
@@ -1548,7 +1642,7 @@
       </c>
       <c r="Z8" s="9">
         <f>SUM(Z2:Z6)</f>
-        <v>4.9547500000000007</v>
+        <v>6.1732499999999995</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
@@ -1557,7 +1651,7 @@
       </c>
       <c r="Z9" s="22">
         <f>SUM(Y2:Y6)+INT(W2/AG15)*AF15+INT(W3/AG16)*AF16+INT(W4/AG17)*AF17+INT(W5/AG18)*AF18+INT(W6/AG19)*AF19</f>
-        <v>20.565833333333334</v>
+        <v>17.912500000000001</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
@@ -1636,7 +1730,7 @@
         <v>21</v>
       </c>
       <c r="Z12">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
@@ -1851,11 +1945,907 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CEA69A-D98C-4A31-9599-286FAD3E94CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG21"/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="J1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="AC8" sqref="AC8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="23" max="23" width="17.33203125" customWidth="1"/>
+    <col min="24" max="24" width="18.44140625" customWidth="1"/>
+    <col min="25" max="25" width="17.44140625" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>1</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="11">
+        <v>0</v>
+      </c>
+      <c r="N2" s="11">
+        <v>0</v>
+      </c>
+      <c r="O2" s="11">
+        <v>0</v>
+      </c>
+      <c r="P2" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>1</v>
+      </c>
+      <c r="R2" s="11">
+        <v>1</v>
+      </c>
+      <c r="S2" s="11">
+        <v>0</v>
+      </c>
+      <c r="T2" s="11">
+        <v>0</v>
+      </c>
+      <c r="U2" s="11">
+        <v>1</v>
+      </c>
+      <c r="V2" s="12">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <f>SUM(C2:V2)</f>
+        <v>5</v>
+      </c>
+      <c r="X2">
+        <f>SUMPRODUCT(C2:V2,B13:U13)</f>
+        <v>8.43</v>
+      </c>
+      <c r="Y2">
+        <f>X2/AC15</f>
+        <v>8.43</v>
+      </c>
+      <c r="Z2">
+        <f>Y2*AD15</f>
+        <v>1.2645</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="13">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <f>SUM(C3:V3)</f>
+        <v>5</v>
+      </c>
+      <c r="X3">
+        <f>SUMPRODUCT(C3:V3,B13:U13)</f>
+        <v>10.609999999999998</v>
+      </c>
+      <c r="Y3">
+        <f>X3/AC16</f>
+        <v>5.3049999999999988</v>
+      </c>
+      <c r="Z3">
+        <f>Y3*AD16</f>
+        <v>1.5914999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0</v>
+      </c>
+      <c r="L4" s="8">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="V4" s="13">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <f>SUM(C4:V4)</f>
+        <v>5</v>
+      </c>
+      <c r="X4">
+        <f>SUMPRODUCT(C4:V4,B13:U13)</f>
+        <v>4.38</v>
+      </c>
+      <c r="Y4">
+        <f>X4/AC17</f>
+        <v>1.46</v>
+      </c>
+      <c r="Z4">
+        <f>Y4*AD17</f>
+        <v>0.65700000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0</v>
+      </c>
+      <c r="V5" s="13">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <f>SUM(C5:V5)</f>
+        <v>4</v>
+      </c>
+      <c r="X5">
+        <f>SUMPRODUCT(C5:V5,B13:U13)</f>
+        <v>6.3800000000000008</v>
+      </c>
+      <c r="Y5">
+        <f>X5/AC18</f>
+        <v>1.5950000000000002</v>
+      </c>
+      <c r="Z5">
+        <f>Y5*AD18</f>
+        <v>1.5950000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16">
+        <v>0</v>
+      </c>
+      <c r="I6" s="16">
+        <v>0</v>
+      </c>
+      <c r="J6" s="16">
+        <v>1</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0</v>
+      </c>
+      <c r="L6" s="16">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <v>0</v>
+      </c>
+      <c r="O6" s="16">
+        <v>0</v>
+      </c>
+      <c r="P6" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="16">
+        <v>0</v>
+      </c>
+      <c r="R6" s="16">
+        <v>0</v>
+      </c>
+      <c r="S6" s="16">
+        <v>0</v>
+      </c>
+      <c r="T6" s="16">
+        <v>0</v>
+      </c>
+      <c r="U6" s="16">
+        <v>0</v>
+      </c>
+      <c r="V6" s="17">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <f>SUM(C6:V6)</f>
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <f>SUMPRODUCT(C6:V6,B13:U13)</f>
+        <v>0.92</v>
+      </c>
+      <c r="Y6">
+        <f>X6/AC18</f>
+        <v>0.23</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" ref="Z6" si="0">Y6*AD19</f>
+        <v>0.34500000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f t="shared" ref="C7:H7" si="1">SUM(C2:C6)</f>
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f>SUM(I2:I6)</f>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7:X7" si="2">SUM(J2:J6)</f>
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="2"/>
+        <v>30.72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Y8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="9">
+        <f>SUM(Z2:Z6)</f>
+        <v>5.4530000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Y9" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z9" s="22">
+        <f>SUM(Y2:Y6)+INT(W2/AG15)*AF15+INT(W3/AG16)*AF16+INT(W4/AG17)*AF17+INT(W5/AG18)*AF18+INT(W6/AG19)*AF19</f>
+        <v>18.22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Y11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <v>9</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>11</v>
+      </c>
+      <c r="M12">
+        <v>12</v>
+      </c>
+      <c r="N12">
+        <v>13</v>
+      </c>
+      <c r="O12">
+        <v>14</v>
+      </c>
+      <c r="P12">
+        <v>15</v>
+      </c>
+      <c r="Q12">
+        <v>16</v>
+      </c>
+      <c r="R12">
+        <v>17</v>
+      </c>
+      <c r="S12">
+        <v>18</v>
+      </c>
+      <c r="T12">
+        <v>19</v>
+      </c>
+      <c r="U12">
+        <v>20</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>1.99</v>
+      </c>
+      <c r="C13">
+        <v>1.93</v>
+      </c>
+      <c r="D13">
+        <v>0.75</v>
+      </c>
+      <c r="E13">
+        <v>0.42</v>
+      </c>
+      <c r="F13">
+        <v>2.57</v>
+      </c>
+      <c r="G13">
+        <v>1.31</v>
+      </c>
+      <c r="H13">
+        <v>1.92</v>
+      </c>
+      <c r="I13">
+        <v>0.92</v>
+      </c>
+      <c r="J13">
+        <v>0.1</v>
+      </c>
+      <c r="K13">
+        <v>3.21</v>
+      </c>
+      <c r="L13">
+        <v>1.53</v>
+      </c>
+      <c r="M13">
+        <v>0.15</v>
+      </c>
+      <c r="N13">
+        <v>2.89</v>
+      </c>
+      <c r="O13">
+        <v>0.95</v>
+      </c>
+      <c r="P13">
+        <v>2.79</v>
+      </c>
+      <c r="Q13">
+        <v>1.06</v>
+      </c>
+      <c r="R13">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="S13">
+        <v>0.61</v>
+      </c>
+      <c r="T13">
+        <v>1.44</v>
+      </c>
+      <c r="U13">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AC14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AB15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>5</v>
+      </c>
+      <c r="AF15" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="AG15" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <f>SUM(B13:U13)</f>
+        <v>30.72</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>2</v>
+      </c>
+      <c r="AD16" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AE16" s="2">
+        <v>5</v>
+      </c>
+      <c r="AF16" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AG16" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="5:33" x14ac:dyDescent="0.3">
+      <c r="AB17" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="AE17" s="2">
+        <v>5</v>
+      </c>
+      <c r="AF17" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="AG17" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="5:33" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="AB18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC18" s="21">
+        <v>4</v>
+      </c>
+      <c r="AD18" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE18" s="19">
+        <v>6</v>
+      </c>
+      <c r="AF18" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AG18" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="5:33" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AB19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC19" s="21">
+        <v>5</v>
+      </c>
+      <c r="AD19" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="AE19" s="19">
+        <v>10</v>
+      </c>
+      <c r="AF19" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="AG19" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="5:33" x14ac:dyDescent="0.3">
+      <c r="AC21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD21">
+        <f>SUM(AE15:AE19)</f>
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>